<commit_message>
celdas amarillas en corte
</commit_message>
<xml_diff>
--- a/public_html/admin/reportesgenerados/EnrollmentFees-87.xlsx
+++ b/public_html/admin/reportesgenerados/EnrollmentFees-87.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="44">
   <si>
     <r>
       <t xml:space="preserve">Renaissance</t>
@@ -55,7 +55,7 @@
     <t>Reflects "Received Revenues" thru:</t>
   </si>
   <si>
-    <t>03/16/2016</t>
+    <t>03/31/2016</t>
   </si>
   <si>
     <t>Enrollment Fees</t>
@@ -163,6 +163,12 @@
   </si>
   <si>
     <t>03/01/2016</t>
+  </si>
+  <si>
+    <t>PE-01-06-17</t>
+  </si>
+  <si>
+    <t>03/19/2016</t>
   </si>
   <si>
     <r>
@@ -1604,9 +1610,15 @@
       <c r="E11" s="12"/>
       <c r="F11" s="13"/>
       <c r="G11" s="14"/>
-      <c r="I11" s="12"/>
-      <c r="J11" s="13"/>
-      <c r="K11" s="14"/>
+      <c r="I11" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="J11" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="K11" s="14">
+        <v>740</v>
+      </c>
       <c r="M11" s="12"/>
       <c r="N11" s="13"/>
       <c r="O11" s="14"/>
@@ -1809,7 +1821,7 @@
     </row>
     <row r="26" spans="1:16" customHeight="1" ht="17.25">
       <c r="A26" s="36" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B26" s="37"/>
       <c r="C26" s="25" t="str">
@@ -1817,7 +1829,7 @@
         <v>0</v>
       </c>
       <c r="E26" s="38" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="F26" s="38"/>
       <c r="G26" s="25" t="str">
@@ -1825,7 +1837,7 @@
         <v>0</v>
       </c>
       <c r="I26" s="36" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="J26" s="36"/>
       <c r="K26" s="25" t="str">
@@ -1833,7 +1845,7 @@
         <v>0</v>
       </c>
       <c r="M26" s="36" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="N26" s="36"/>
       <c r="O26" s="25" t="str">
@@ -1844,22 +1856,22 @@
     <row r="27" spans="1:16" customHeight="1" ht="17.25"/>
     <row r="28" spans="1:16" customHeight="1" ht="17.25">
       <c r="A28" s="33" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="B28" s="34"/>
       <c r="C28" s="35"/>
       <c r="E28" s="33" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="F28" s="34"/>
       <c r="G28" s="35"/>
       <c r="I28" s="33" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="J28" s="34"/>
       <c r="K28" s="35"/>
       <c r="M28" s="33" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="N28" s="34"/>
       <c r="O28" s="35"/>
@@ -2166,7 +2178,7 @@
     </row>
     <row r="47" spans="1:16" customHeight="1" ht="17.25">
       <c r="A47" s="36" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B47" s="36"/>
       <c r="C47" s="25" t="str">
@@ -2174,7 +2186,7 @@
         <v>0</v>
       </c>
       <c r="E47" s="36" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="F47" s="36"/>
       <c r="G47" s="25" t="str">
@@ -2182,7 +2194,7 @@
         <v>0</v>
       </c>
       <c r="I47" s="36" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="J47" s="36"/>
       <c r="K47" s="25" t="str">
@@ -2190,7 +2202,7 @@
         <v>0</v>
       </c>
       <c r="M47" s="36" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="N47" s="36"/>
       <c r="O47" s="25" t="str">
@@ -2201,22 +2213,22 @@
     <row r="48" spans="1:16" customHeight="1" ht="17.25"/>
     <row r="49" spans="1:16" customHeight="1" ht="17.25">
       <c r="A49" s="33" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="B49" s="34"/>
       <c r="C49" s="35"/>
       <c r="E49" s="33" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="F49" s="34"/>
       <c r="G49" s="35"/>
       <c r="I49" s="33" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="J49" s="34"/>
       <c r="K49" s="35"/>
       <c r="M49" s="33" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="N49" s="34"/>
       <c r="O49" s="35"/>
@@ -2523,7 +2535,7 @@
     </row>
     <row r="68" spans="1:16" customHeight="1" ht="17.25">
       <c r="A68" s="36" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="B68" s="36"/>
       <c r="C68" s="25" t="str">
@@ -2531,7 +2543,7 @@
         <v>0</v>
       </c>
       <c r="E68" s="36" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="F68" s="36"/>
       <c r="G68" s="25" t="str">
@@ -2539,7 +2551,7 @@
         <v>0</v>
       </c>
       <c r="I68" s="36" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="J68" s="36"/>
       <c r="K68" s="25" t="str">
@@ -2547,7 +2559,7 @@
         <v>0</v>
       </c>
       <c r="M68" s="36" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="N68" s="36"/>
       <c r="O68" s="25" t="str">
@@ -2900,7 +2912,7 @@
     </row>
     <row r="93" spans="1:16" customHeight="1" ht="17.25">
       <c r="A93" s="36" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="B93" s="36"/>
       <c r="C93" s="25" t="str">
@@ -2908,7 +2920,7 @@
         <v>0</v>
       </c>
       <c r="E93" s="38" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="F93" s="38"/>
       <c r="G93" s="25" t="str">
@@ -2916,7 +2928,7 @@
         <v>0</v>
       </c>
       <c r="I93" s="36" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="J93" s="36"/>
       <c r="K93" s="25" t="str">
@@ -2924,7 +2936,7 @@
         <v>0</v>
       </c>
       <c r="M93" s="36" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="N93" s="36"/>
       <c r="O93" s="25" t="str">

</xml_diff>

<commit_message>
reporte generando hojas dinamicamente
</commit_message>
<xml_diff>
--- a/public_html/admin/reportesgenerados/EnrollmentFees-87.xlsx
+++ b/public_html/admin/reportesgenerados/EnrollmentFees-87.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="36">
   <si>
     <r>
       <t xml:space="preserve">Renaissance</t>
@@ -147,117 +147,6 @@
     <t>Amount</t>
   </si>
   <si>
-    <t>PE-01-02-53</t>
-  </si>
-  <si>
-    <t>01/27/2017</t>
-  </si>
-  <si>
-    <t>PE-01-04-29</t>
-  </si>
-  <si>
-    <t>02/22/2017</t>
-  </si>
-  <si>
-    <t>PE-01-05-27</t>
-  </si>
-  <si>
-    <t>03/24/2017</t>
-  </si>
-  <si>
-    <t>PE-01-02-54</t>
-  </si>
-  <si>
-    <t>04/19/2017</t>
-  </si>
-  <si>
-    <t>PE-01-06-22</t>
-  </si>
-  <si>
-    <t>02/01/2017</t>
-  </si>
-  <si>
-    <t>PE-01-06-23</t>
-  </si>
-  <si>
-    <t>PE-01-06-26</t>
-  </si>
-  <si>
-    <t>04/21/2017</t>
-  </si>
-  <si>
-    <t>PE-01-07-17</t>
-  </si>
-  <si>
-    <t>02/23/2017</t>
-  </si>
-  <si>
-    <t>PE-01-06-24</t>
-  </si>
-  <si>
-    <t>03/01/2017</t>
-  </si>
-  <si>
-    <t>PE-01-10-06</t>
-  </si>
-  <si>
-    <t>04/18/2017</t>
-  </si>
-  <si>
-    <t>PE-01-08-16</t>
-  </si>
-  <si>
-    <t>PE-01-07-22</t>
-  </si>
-  <si>
-    <t>03/16/2017</t>
-  </si>
-  <si>
-    <t>PE-01-08-17</t>
-  </si>
-  <si>
-    <t>02/24/2017</t>
-  </si>
-  <si>
-    <t>PE-01-07-26</t>
-  </si>
-  <si>
-    <t>03/23/2017</t>
-  </si>
-  <si>
-    <t>PE-01-09-12</t>
-  </si>
-  <si>
-    <t>02/20/2017</t>
-  </si>
-  <si>
-    <t>PE-01-10-08</t>
-  </si>
-  <si>
-    <t>03/02/2017</t>
-  </si>
-  <si>
-    <t>PE-01-10-01</t>
-  </si>
-  <si>
-    <t>02/17/2017</t>
-  </si>
-  <si>
-    <t>PE-01-10-02</t>
-  </si>
-  <si>
-    <t>02/13/2017</t>
-  </si>
-  <si>
-    <t>PE-01-10-04</t>
-  </si>
-  <si>
-    <t>02/14/2017</t>
-  </si>
-  <si>
-    <t>PE-01-10-05</t>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">TOTAL FOR </t>
     </r>
@@ -404,45 +293,6 @@
       </rPr>
       <t xml:space="preserve">AUGUST</t>
     </r>
-  </si>
-  <si>
-    <t>PE-01-01-42</t>
-  </si>
-  <si>
-    <t>05/19/2017</t>
-  </si>
-  <si>
-    <t>PE-01-09-13</t>
-  </si>
-  <si>
-    <t>06/13/2017</t>
-  </si>
-  <si>
-    <t>PE-01-04-30</t>
-  </si>
-  <si>
-    <t>05/24/2017</t>
-  </si>
-  <si>
-    <t>PE-01-07-29</t>
-  </si>
-  <si>
-    <t>05/23/2017</t>
-  </si>
-  <si>
-    <t>PE-01-10-09</t>
-  </si>
-  <si>
-    <t>05/05/2017</t>
-  </si>
-  <si>
-    <t>PE-01-10-10</t>
-  </si>
-  <si>
-    <t>05/04/2017</t>
-  </si>
-  <si>
-    <t>PE-01-10-11</t>
   </si>
   <si>
     <r>
@@ -1698,129 +1548,57 @@
       </c>
     </row>
     <row r="10" spans="1:16">
-      <c r="A10" s="12" t="s">
-        <v>16</v>
-      </c>
-      <c r="B10" s="13" t="s">
-        <v>17</v>
-      </c>
-      <c r="C10" s="14">
-        <v>740</v>
-      </c>
-      <c r="E10" s="12" t="s">
-        <v>18</v>
-      </c>
-      <c r="F10" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="G10" s="14">
-        <v>780</v>
-      </c>
-      <c r="I10" s="12" t="s">
-        <v>20</v>
-      </c>
-      <c r="J10" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="K10" s="14">
-        <v>780</v>
-      </c>
-      <c r="M10" s="12" t="s">
-        <v>22</v>
-      </c>
-      <c r="N10" s="13" t="s">
-        <v>23</v>
-      </c>
-      <c r="O10" s="14">
-        <v>780</v>
-      </c>
+      <c r="A10" s="12"/>
+      <c r="B10" s="13"/>
+      <c r="C10" s="14"/>
+      <c r="E10" s="12"/>
+      <c r="F10" s="13"/>
+      <c r="G10" s="14"/>
+      <c r="I10" s="12"/>
+      <c r="J10" s="13"/>
+      <c r="K10" s="14"/>
+      <c r="M10" s="12"/>
+      <c r="N10" s="13"/>
+      <c r="O10" s="14"/>
     </row>
     <row r="11" spans="1:16">
       <c r="A11" s="15"/>
       <c r="B11" s="16"/>
       <c r="C11" s="14"/>
-      <c r="E11" s="12" t="s">
-        <v>24</v>
-      </c>
-      <c r="F11" s="13" t="s">
-        <v>25</v>
-      </c>
-      <c r="G11" s="14">
-        <v>740</v>
-      </c>
-      <c r="I11" s="12" t="s">
-        <v>26</v>
-      </c>
-      <c r="J11" s="13" t="s">
-        <v>21</v>
-      </c>
-      <c r="K11" s="14">
-        <v>780</v>
-      </c>
-      <c r="M11" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="N11" s="13" t="s">
-        <v>28</v>
-      </c>
-      <c r="O11" s="14">
-        <v>780</v>
-      </c>
+      <c r="E11" s="12"/>
+      <c r="F11" s="13"/>
+      <c r="G11" s="14"/>
+      <c r="I11" s="12"/>
+      <c r="J11" s="13"/>
+      <c r="K11" s="14"/>
+      <c r="M11" s="12"/>
+      <c r="N11" s="13"/>
+      <c r="O11" s="14"/>
     </row>
     <row r="12" spans="1:16">
       <c r="A12" s="15"/>
       <c r="B12" s="16"/>
       <c r="C12" s="14"/>
-      <c r="E12" s="12" t="s">
-        <v>29</v>
-      </c>
-      <c r="F12" s="16" t="s">
-        <v>30</v>
-      </c>
-      <c r="G12" s="14">
-        <v>740</v>
-      </c>
-      <c r="I12" s="12" t="s">
-        <v>31</v>
-      </c>
-      <c r="J12" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="K12" s="14">
-        <v>780</v>
-      </c>
-      <c r="M12" s="12" t="s">
-        <v>33</v>
-      </c>
-      <c r="N12" s="13" t="s">
-        <v>34</v>
-      </c>
-      <c r="O12" s="14">
-        <v>740</v>
-      </c>
+      <c r="E12" s="12"/>
+      <c r="F12" s="16"/>
+      <c r="G12" s="14"/>
+      <c r="I12" s="12"/>
+      <c r="J12" s="13"/>
+      <c r="K12" s="14"/>
+      <c r="M12" s="12"/>
+      <c r="N12" s="13"/>
+      <c r="O12" s="14"/>
     </row>
     <row r="13" spans="1:16">
       <c r="A13" s="15"/>
       <c r="B13" s="16"/>
       <c r="C13" s="17"/>
-      <c r="E13" s="12" t="s">
-        <v>35</v>
-      </c>
-      <c r="F13" s="16" t="s">
-        <v>25</v>
-      </c>
-      <c r="G13" s="17">
-        <v>740</v>
-      </c>
-      <c r="I13" s="12" t="s">
-        <v>36</v>
-      </c>
-      <c r="J13" s="13" t="s">
-        <v>37</v>
-      </c>
-      <c r="K13" s="17">
-        <v>740</v>
-      </c>
+      <c r="E13" s="12"/>
+      <c r="F13" s="16"/>
+      <c r="G13" s="17"/>
+      <c r="I13" s="12"/>
+      <c r="J13" s="13"/>
+      <c r="K13" s="17"/>
       <c r="M13" s="15"/>
       <c r="N13" s="16"/>
       <c r="O13" s="17"/>
@@ -1829,24 +1607,12 @@
       <c r="A14" s="15"/>
       <c r="B14" s="16"/>
       <c r="C14" s="14"/>
-      <c r="E14" s="15" t="s">
-        <v>38</v>
-      </c>
-      <c r="F14" s="16" t="s">
-        <v>39</v>
-      </c>
-      <c r="G14" s="14">
-        <v>780</v>
-      </c>
-      <c r="I14" s="15" t="s">
-        <v>40</v>
-      </c>
-      <c r="J14" s="18" t="s">
-        <v>41</v>
-      </c>
-      <c r="K14" s="14">
-        <v>740</v>
-      </c>
+      <c r="E14" s="15"/>
+      <c r="F14" s="16"/>
+      <c r="G14" s="14"/>
+      <c r="I14" s="15"/>
+      <c r="J14" s="18"/>
+      <c r="K14" s="14"/>
       <c r="M14" s="15"/>
       <c r="N14" s="16"/>
       <c r="O14" s="14"/>
@@ -1855,24 +1621,12 @@
       <c r="A15" s="15"/>
       <c r="B15" s="16"/>
       <c r="C15" s="14"/>
-      <c r="E15" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="F15" s="16" t="s">
-        <v>43</v>
-      </c>
-      <c r="G15" s="14">
-        <v>740</v>
-      </c>
-      <c r="I15" s="15" t="s">
-        <v>44</v>
-      </c>
-      <c r="J15" s="18" t="s">
-        <v>45</v>
-      </c>
-      <c r="K15" s="14">
-        <v>520</v>
-      </c>
+      <c r="E15" s="15"/>
+      <c r="F15" s="16"/>
+      <c r="G15" s="14"/>
+      <c r="I15" s="15"/>
+      <c r="J15" s="18"/>
+      <c r="K15" s="14"/>
       <c r="M15" s="15"/>
       <c r="N15" s="16"/>
       <c r="O15" s="14"/>
@@ -1881,15 +1635,9 @@
       <c r="A16" s="15"/>
       <c r="B16" s="16"/>
       <c r="C16" s="17"/>
-      <c r="E16" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="F16" s="16" t="s">
-        <v>47</v>
-      </c>
-      <c r="G16" s="17">
-        <v>780</v>
-      </c>
+      <c r="E16" s="15"/>
+      <c r="F16" s="16"/>
+      <c r="G16" s="17"/>
       <c r="I16" s="15"/>
       <c r="J16" s="16"/>
       <c r="K16" s="17"/>
@@ -1901,15 +1649,9 @@
       <c r="A17" s="19"/>
       <c r="B17" s="20"/>
       <c r="C17" s="21"/>
-      <c r="E17" s="19" t="s">
-        <v>48</v>
-      </c>
-      <c r="F17" s="20" t="s">
-        <v>49</v>
-      </c>
-      <c r="G17" s="21">
-        <v>780</v>
-      </c>
+      <c r="E17" s="19"/>
+      <c r="F17" s="20"/>
+      <c r="G17" s="21"/>
       <c r="I17" s="19"/>
       <c r="J17" s="20"/>
       <c r="K17" s="21"/>
@@ -1921,15 +1663,9 @@
       <c r="A18" s="19"/>
       <c r="B18" s="20"/>
       <c r="C18" s="21"/>
-      <c r="E18" s="19" t="s">
-        <v>50</v>
-      </c>
-      <c r="F18" s="20" t="s">
-        <v>51</v>
-      </c>
-      <c r="G18" s="21">
-        <v>780</v>
-      </c>
+      <c r="E18" s="19"/>
+      <c r="F18" s="20"/>
+      <c r="G18" s="21"/>
       <c r="I18" s="19"/>
       <c r="J18" s="20"/>
       <c r="K18" s="21"/>
@@ -1941,15 +1677,9 @@
       <c r="A19" s="19"/>
       <c r="B19" s="20"/>
       <c r="C19" s="21"/>
-      <c r="E19" s="19" t="s">
-        <v>52</v>
-      </c>
-      <c r="F19" s="20" t="s">
-        <v>39</v>
-      </c>
-      <c r="G19" s="21">
-        <v>780</v>
-      </c>
+      <c r="E19" s="19"/>
+      <c r="F19" s="20"/>
+      <c r="G19" s="21"/>
       <c r="I19" s="19"/>
       <c r="J19" s="20"/>
       <c r="K19" s="21"/>
@@ -2043,7 +1773,7 @@
     </row>
     <row r="26" spans="1:16" customHeight="1" ht="17.25">
       <c r="A26" s="36" t="s">
-        <v>53</v>
+        <v>16</v>
       </c>
       <c r="B26" s="37"/>
       <c r="C26" s="25" t="str">
@@ -2051,7 +1781,7 @@
         <v>0</v>
       </c>
       <c r="E26" s="38" t="s">
-        <v>54</v>
+        <v>17</v>
       </c>
       <c r="F26" s="38"/>
       <c r="G26" s="25" t="str">
@@ -2059,7 +1789,7 @@
         <v>0</v>
       </c>
       <c r="I26" s="36" t="s">
-        <v>55</v>
+        <v>18</v>
       </c>
       <c r="J26" s="36"/>
       <c r="K26" s="25" t="str">
@@ -2067,7 +1797,7 @@
         <v>0</v>
       </c>
       <c r="M26" s="36" t="s">
-        <v>56</v>
+        <v>19</v>
       </c>
       <c r="N26" s="36"/>
       <c r="O26" s="25" t="str">
@@ -2078,22 +1808,22 @@
     <row r="27" spans="1:16" customHeight="1" ht="17.25"/>
     <row r="28" spans="1:16" customHeight="1" ht="17.25">
       <c r="A28" s="33" t="s">
-        <v>57</v>
+        <v>20</v>
       </c>
       <c r="B28" s="34"/>
       <c r="C28" s="35"/>
       <c r="E28" s="33" t="s">
-        <v>58</v>
+        <v>21</v>
       </c>
       <c r="F28" s="34"/>
       <c r="G28" s="35"/>
       <c r="I28" s="33" t="s">
-        <v>59</v>
+        <v>22</v>
       </c>
       <c r="J28" s="34"/>
       <c r="K28" s="35"/>
       <c r="M28" s="33" t="s">
-        <v>60</v>
+        <v>23</v>
       </c>
       <c r="N28" s="34"/>
       <c r="O28" s="35"/>
@@ -2175,24 +1905,12 @@
       </c>
     </row>
     <row r="31" spans="1:16">
-      <c r="A31" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="B31" s="13" t="s">
-        <v>62</v>
-      </c>
-      <c r="C31" s="14">
-        <v>780</v>
-      </c>
-      <c r="E31" s="12" t="s">
-        <v>63</v>
-      </c>
-      <c r="F31" s="13" t="s">
-        <v>64</v>
-      </c>
-      <c r="G31" s="14">
-        <v>780</v>
-      </c>
+      <c r="A31" s="12"/>
+      <c r="B31" s="13"/>
+      <c r="C31" s="14"/>
+      <c r="E31" s="12"/>
+      <c r="F31" s="13"/>
+      <c r="G31" s="14"/>
       <c r="I31" s="12"/>
       <c r="J31" s="13"/>
       <c r="K31" s="14"/>
@@ -2201,15 +1919,9 @@
       <c r="O31" s="14"/>
     </row>
     <row r="32" spans="1:16">
-      <c r="A32" s="12" t="s">
-        <v>65</v>
-      </c>
-      <c r="B32" s="13" t="s">
-        <v>66</v>
-      </c>
-      <c r="C32" s="14">
-        <v>780</v>
-      </c>
+      <c r="A32" s="12"/>
+      <c r="B32" s="13"/>
+      <c r="C32" s="14"/>
       <c r="E32" s="12"/>
       <c r="F32" s="13"/>
       <c r="G32" s="14"/>
@@ -2221,15 +1933,9 @@
       <c r="O32" s="14"/>
     </row>
     <row r="33" spans="1:16">
-      <c r="A33" s="12" t="s">
-        <v>67</v>
-      </c>
-      <c r="B33" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="C33" s="14">
-        <v>780</v>
-      </c>
+      <c r="A33" s="12"/>
+      <c r="B33" s="13"/>
+      <c r="C33" s="14"/>
       <c r="E33" s="26"/>
       <c r="F33" s="13"/>
       <c r="G33" s="14"/>
@@ -2241,15 +1947,9 @@
       <c r="O33" s="14"/>
     </row>
     <row r="34" spans="1:16">
-      <c r="A34" s="15" t="s">
-        <v>69</v>
-      </c>
-      <c r="B34" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="C34" s="17">
-        <v>780</v>
-      </c>
+      <c r="A34" s="15"/>
+      <c r="B34" s="16"/>
+      <c r="C34" s="17"/>
       <c r="E34" s="15"/>
       <c r="F34" s="16"/>
       <c r="G34" s="17"/>
@@ -2261,15 +1961,9 @@
       <c r="O34" s="17"/>
     </row>
     <row r="35" spans="1:16">
-      <c r="A35" s="15" t="s">
-        <v>71</v>
-      </c>
-      <c r="B35" s="16" t="s">
-        <v>72</v>
-      </c>
-      <c r="C35" s="14">
-        <v>780</v>
-      </c>
+      <c r="A35" s="15"/>
+      <c r="B35" s="16"/>
+      <c r="C35" s="14"/>
       <c r="E35" s="26"/>
       <c r="F35" s="13"/>
       <c r="G35" s="14"/>
@@ -2281,15 +1975,9 @@
       <c r="O35" s="14"/>
     </row>
     <row r="36" spans="1:16">
-      <c r="A36" s="15" t="s">
-        <v>73</v>
-      </c>
-      <c r="B36" s="16" t="s">
-        <v>70</v>
-      </c>
-      <c r="C36" s="14">
-        <v>780</v>
-      </c>
+      <c r="A36" s="15"/>
+      <c r="B36" s="16"/>
+      <c r="C36" s="14"/>
       <c r="E36" s="26"/>
       <c r="F36" s="13"/>
       <c r="G36" s="14"/>
@@ -2442,7 +2130,7 @@
     </row>
     <row r="47" spans="1:16" customHeight="1" ht="17.25">
       <c r="A47" s="36" t="s">
-        <v>74</v>
+        <v>24</v>
       </c>
       <c r="B47" s="36"/>
       <c r="C47" s="25" t="str">
@@ -2450,7 +2138,7 @@
         <v>0</v>
       </c>
       <c r="E47" s="36" t="s">
-        <v>75</v>
+        <v>25</v>
       </c>
       <c r="F47" s="36"/>
       <c r="G47" s="25" t="str">
@@ -2458,7 +2146,7 @@
         <v>0</v>
       </c>
       <c r="I47" s="36" t="s">
-        <v>76</v>
+        <v>26</v>
       </c>
       <c r="J47" s="36"/>
       <c r="K47" s="25" t="str">
@@ -2466,7 +2154,7 @@
         <v>0</v>
       </c>
       <c r="M47" s="36" t="s">
-        <v>77</v>
+        <v>27</v>
       </c>
       <c r="N47" s="36"/>
       <c r="O47" s="25" t="str">
@@ -2477,22 +2165,22 @@
     <row r="48" spans="1:16" customHeight="1" ht="17.25"/>
     <row r="49" spans="1:16" customHeight="1" ht="17.25">
       <c r="A49" s="33" t="s">
-        <v>78</v>
+        <v>28</v>
       </c>
       <c r="B49" s="34"/>
       <c r="C49" s="35"/>
       <c r="E49" s="33" t="s">
-        <v>79</v>
+        <v>29</v>
       </c>
       <c r="F49" s="34"/>
       <c r="G49" s="35"/>
       <c r="I49" s="33" t="s">
-        <v>80</v>
+        <v>30</v>
       </c>
       <c r="J49" s="34"/>
       <c r="K49" s="35"/>
       <c r="M49" s="33" t="s">
-        <v>81</v>
+        <v>31</v>
       </c>
       <c r="N49" s="34"/>
       <c r="O49" s="35"/>
@@ -2799,7 +2487,7 @@
     </row>
     <row r="68" spans="1:16" customHeight="1" ht="17.25">
       <c r="A68" s="36" t="s">
-        <v>82</v>
+        <v>32</v>
       </c>
       <c r="B68" s="36"/>
       <c r="C68" s="25" t="str">
@@ -2807,7 +2495,7 @@
         <v>0</v>
       </c>
       <c r="E68" s="36" t="s">
-        <v>83</v>
+        <v>33</v>
       </c>
       <c r="F68" s="36"/>
       <c r="G68" s="25" t="str">
@@ -2815,7 +2503,7 @@
         <v>0</v>
       </c>
       <c r="I68" s="36" t="s">
-        <v>84</v>
+        <v>34</v>
       </c>
       <c r="J68" s="36"/>
       <c r="K68" s="25" t="str">
@@ -2823,7 +2511,7 @@
         <v>0</v>
       </c>
       <c r="M68" s="36" t="s">
-        <v>85</v>
+        <v>35</v>
       </c>
       <c r="N68" s="36"/>
       <c r="O68" s="25" t="str">
@@ -2834,7 +2522,7 @@
     <row r="71" spans="1:16" customHeight="1" ht="17.25"/>
     <row r="72" spans="1:16" customHeight="1" ht="27.75">
       <c r="A72" s="39">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="B72" s="40"/>
       <c r="C72" s="40"/>
@@ -3176,7 +2864,7 @@
     </row>
     <row r="93" spans="1:16" customHeight="1" ht="17.25">
       <c r="A93" s="36" t="s">
-        <v>53</v>
+        <v>16</v>
       </c>
       <c r="B93" s="36"/>
       <c r="C93" s="25" t="str">
@@ -3184,7 +2872,7 @@
         <v>0</v>
       </c>
       <c r="E93" s="38" t="s">
-        <v>54</v>
+        <v>17</v>
       </c>
       <c r="F93" s="38"/>
       <c r="G93" s="25" t="str">
@@ -3192,7 +2880,7 @@
         <v>0</v>
       </c>
       <c r="I93" s="36" t="s">
-        <v>55</v>
+        <v>18</v>
       </c>
       <c r="J93" s="36"/>
       <c r="K93" s="25" t="str">
@@ -3200,7 +2888,7 @@
         <v>0</v>
       </c>
       <c r="M93" s="36" t="s">
-        <v>56</v>
+        <v>19</v>
       </c>
       <c r="N93" s="36"/>
       <c r="O93" s="25" t="str">
@@ -3208,7 +2896,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="95" spans="1:16">
+    <row r="94" spans="1:16" hidden="true"/>
+    <row r="95" spans="1:16" hidden="true">
       <c r="A95" s="42"/>
       <c r="B95" s="42"/>
       <c r="C95" s="42"/>
@@ -3226,7 +2915,7 @@
       <c r="O95" s="42"/>
       <c r="P95" s="44"/>
     </row>
-    <row r="96" spans="1:16">
+    <row r="96" spans="1:16" hidden="true">
       <c r="A96" s="45"/>
       <c r="B96" s="45"/>
       <c r="C96" s="45"/>
@@ -3244,7 +2933,7 @@
       <c r="O96" s="45"/>
       <c r="P96" s="44"/>
     </row>
-    <row r="97" spans="1:16">
+    <row r="97" spans="1:16" hidden="true">
       <c r="A97" s="45"/>
       <c r="B97" s="45"/>
       <c r="C97" s="45"/>
@@ -3262,7 +2951,7 @@
       <c r="O97" s="45"/>
       <c r="P97" s="44"/>
     </row>
-    <row r="98" spans="1:16">
+    <row r="98" spans="1:16" hidden="true">
       <c r="A98" s="43"/>
       <c r="B98" s="46"/>
       <c r="C98" s="47"/>
@@ -3280,7 +2969,7 @@
       <c r="O98" s="47"/>
       <c r="P98" s="44"/>
     </row>
-    <row r="99" spans="1:16">
+    <row r="99" spans="1:16" hidden="true">
       <c r="A99" s="43"/>
       <c r="B99" s="46"/>
       <c r="C99" s="47"/>
@@ -3298,7 +2987,7 @@
       <c r="O99" s="47"/>
       <c r="P99" s="44"/>
     </row>
-    <row r="100" spans="1:16">
+    <row r="100" spans="1:16" hidden="true">
       <c r="A100" s="43"/>
       <c r="B100" s="46"/>
       <c r="C100" s="47"/>
@@ -3316,7 +3005,7 @@
       <c r="O100" s="47"/>
       <c r="P100" s="44"/>
     </row>
-    <row r="101" spans="1:16">
+    <row r="101" spans="1:16" hidden="true">
       <c r="A101" s="43"/>
       <c r="B101" s="46"/>
       <c r="C101" s="47"/>
@@ -3334,7 +3023,7 @@
       <c r="O101" s="47"/>
       <c r="P101" s="44"/>
     </row>
-    <row r="102" spans="1:16">
+    <row r="102" spans="1:16" hidden="true">
       <c r="A102" s="43"/>
       <c r="B102" s="46"/>
       <c r="C102" s="47"/>
@@ -3352,7 +3041,7 @@
       <c r="O102" s="47"/>
       <c r="P102" s="44"/>
     </row>
-    <row r="103" spans="1:16">
+    <row r="103" spans="1:16" hidden="true">
       <c r="A103" s="43"/>
       <c r="B103" s="46"/>
       <c r="C103" s="47"/>
@@ -3370,7 +3059,7 @@
       <c r="O103" s="47"/>
       <c r="P103" s="44"/>
     </row>
-    <row r="104" spans="1:16">
+    <row r="104" spans="1:16" hidden="true">
       <c r="A104" s="43"/>
       <c r="B104" s="46"/>
       <c r="C104" s="47"/>
@@ -3388,7 +3077,7 @@
       <c r="O104" s="47"/>
       <c r="P104" s="44"/>
     </row>
-    <row r="105" spans="1:16">
+    <row r="105" spans="1:16" hidden="true">
       <c r="A105" s="43"/>
       <c r="B105" s="46"/>
       <c r="C105" s="47"/>
@@ -3406,7 +3095,7 @@
       <c r="O105" s="47"/>
       <c r="P105" s="44"/>
     </row>
-    <row r="106" spans="1:16">
+    <row r="106" spans="1:16" hidden="true">
       <c r="A106" s="43"/>
       <c r="B106" s="46"/>
       <c r="C106" s="47"/>
@@ -3424,7 +3113,7 @@
       <c r="O106" s="47"/>
       <c r="P106" s="44"/>
     </row>
-    <row r="107" spans="1:16">
+    <row r="107" spans="1:16" hidden="true">
       <c r="A107" s="43"/>
       <c r="B107" s="46"/>
       <c r="C107" s="47"/>
@@ -3442,7 +3131,7 @@
       <c r="O107" s="47"/>
       <c r="P107" s="44"/>
     </row>
-    <row r="108" spans="1:16">
+    <row r="108" spans="1:16" hidden="true">
       <c r="A108" s="43"/>
       <c r="B108" s="46"/>
       <c r="C108" s="47"/>
@@ -3460,7 +3149,7 @@
       <c r="O108" s="47"/>
       <c r="P108" s="44"/>
     </row>
-    <row r="109" spans="1:16">
+    <row r="109" spans="1:16" hidden="true">
       <c r="A109" s="43"/>
       <c r="B109" s="46"/>
       <c r="C109" s="47"/>
@@ -3478,7 +3167,7 @@
       <c r="O109" s="47"/>
       <c r="P109" s="44"/>
     </row>
-    <row r="110" spans="1:16">
+    <row r="110" spans="1:16" hidden="true">
       <c r="A110" s="43"/>
       <c r="B110" s="46"/>
       <c r="C110" s="47"/>
@@ -3496,7 +3185,7 @@
       <c r="O110" s="47"/>
       <c r="P110" s="44"/>
     </row>
-    <row r="111" spans="1:16">
+    <row r="111" spans="1:16" hidden="true">
       <c r="A111" s="43"/>
       <c r="B111" s="46"/>
       <c r="C111" s="47"/>
@@ -3514,7 +3203,7 @@
       <c r="O111" s="47"/>
       <c r="P111" s="44"/>
     </row>
-    <row r="112" spans="1:16">
+    <row r="112" spans="1:16" hidden="true">
       <c r="A112" s="43"/>
       <c r="B112" s="46"/>
       <c r="C112" s="47"/>
@@ -3532,7 +3221,7 @@
       <c r="O112" s="47"/>
       <c r="P112" s="44"/>
     </row>
-    <row r="113" spans="1:16">
+    <row r="113" spans="1:16" hidden="true">
       <c r="A113" s="43"/>
       <c r="B113" s="46"/>
       <c r="C113" s="47"/>
@@ -3550,7 +3239,7 @@
       <c r="O113" s="47"/>
       <c r="P113" s="44"/>
     </row>
-    <row r="114" spans="1:16">
+    <row r="114" spans="1:16" hidden="true">
       <c r="A114" s="49"/>
       <c r="B114" s="49"/>
       <c r="C114" s="47"/>
@@ -3568,7 +3257,7 @@
       <c r="O114" s="47"/>
       <c r="P114" s="44"/>
     </row>
-    <row r="115" spans="1:16">
+    <row r="115" spans="1:16" hidden="true">
       <c r="A115" s="43"/>
       <c r="B115" s="43"/>
       <c r="C115" s="43"/>
@@ -3586,7 +3275,7 @@
       <c r="O115" s="43"/>
       <c r="P115" s="44"/>
     </row>
-    <row r="116" spans="1:16">
+    <row r="116" spans="1:16" hidden="true">
       <c r="A116" s="42"/>
       <c r="B116" s="42"/>
       <c r="C116" s="42"/>
@@ -3604,7 +3293,7 @@
       <c r="O116" s="42"/>
       <c r="P116" s="44"/>
     </row>
-    <row r="117" spans="1:16">
+    <row r="117" spans="1:16" hidden="true">
       <c r="A117" s="45"/>
       <c r="B117" s="45"/>
       <c r="C117" s="45"/>
@@ -3622,7 +3311,7 @@
       <c r="O117" s="45"/>
       <c r="P117" s="44"/>
     </row>
-    <row r="118" spans="1:16">
+    <row r="118" spans="1:16" hidden="true">
       <c r="A118" s="45"/>
       <c r="B118" s="45"/>
       <c r="C118" s="45"/>
@@ -3640,7 +3329,7 @@
       <c r="O118" s="45"/>
       <c r="P118" s="44"/>
     </row>
-    <row r="119" spans="1:16">
+    <row r="119" spans="1:16" hidden="true">
       <c r="A119" s="43"/>
       <c r="B119" s="46"/>
       <c r="C119" s="47"/>
@@ -3658,7 +3347,7 @@
       <c r="O119" s="47"/>
       <c r="P119" s="44"/>
     </row>
-    <row r="120" spans="1:16">
+    <row r="120" spans="1:16" hidden="true">
       <c r="A120" s="43"/>
       <c r="B120" s="46"/>
       <c r="C120" s="47"/>
@@ -3676,7 +3365,7 @@
       <c r="O120" s="47"/>
       <c r="P120" s="44"/>
     </row>
-    <row r="121" spans="1:16">
+    <row r="121" spans="1:16" hidden="true">
       <c r="A121" s="43"/>
       <c r="B121" s="46"/>
       <c r="C121" s="47"/>
@@ -3694,7 +3383,7 @@
       <c r="O121" s="47"/>
       <c r="P121" s="44"/>
     </row>
-    <row r="122" spans="1:16">
+    <row r="122" spans="1:16" hidden="true">
       <c r="A122" s="43"/>
       <c r="B122" s="46"/>
       <c r="C122" s="47"/>
@@ -3712,7 +3401,7 @@
       <c r="O122" s="47"/>
       <c r="P122" s="44"/>
     </row>
-    <row r="123" spans="1:16">
+    <row r="123" spans="1:16" hidden="true">
       <c r="A123" s="43"/>
       <c r="B123" s="46"/>
       <c r="C123" s="47"/>
@@ -3730,7 +3419,7 @@
       <c r="O123" s="47"/>
       <c r="P123" s="44"/>
     </row>
-    <row r="124" spans="1:16">
+    <row r="124" spans="1:16" hidden="true">
       <c r="A124" s="43"/>
       <c r="B124" s="46"/>
       <c r="C124" s="47"/>
@@ -3748,7 +3437,7 @@
       <c r="O124" s="47"/>
       <c r="P124" s="44"/>
     </row>
-    <row r="125" spans="1:16">
+    <row r="125" spans="1:16" hidden="true">
       <c r="A125" s="43"/>
       <c r="B125" s="46"/>
       <c r="C125" s="47"/>
@@ -3766,7 +3455,7 @@
       <c r="O125" s="47"/>
       <c r="P125" s="44"/>
     </row>
-    <row r="126" spans="1:16">
+    <row r="126" spans="1:16" hidden="true">
       <c r="A126" s="43"/>
       <c r="B126" s="46"/>
       <c r="C126" s="47"/>
@@ -3784,7 +3473,7 @@
       <c r="O126" s="47"/>
       <c r="P126" s="44"/>
     </row>
-    <row r="127" spans="1:16">
+    <row r="127" spans="1:16" hidden="true">
       <c r="A127" s="43"/>
       <c r="B127" s="46"/>
       <c r="C127" s="47"/>
@@ -3802,7 +3491,7 @@
       <c r="O127" s="47"/>
       <c r="P127" s="44"/>
     </row>
-    <row r="128" spans="1:16">
+    <row r="128" spans="1:16" hidden="true">
       <c r="A128" s="43"/>
       <c r="B128" s="46"/>
       <c r="C128" s="47"/>
@@ -3820,7 +3509,7 @@
       <c r="O128" s="47"/>
       <c r="P128" s="44"/>
     </row>
-    <row r="129" spans="1:16">
+    <row r="129" spans="1:16" hidden="true">
       <c r="A129" s="43"/>
       <c r="B129" s="46"/>
       <c r="C129" s="47"/>
@@ -3838,7 +3527,7 @@
       <c r="O129" s="47"/>
       <c r="P129" s="44"/>
     </row>
-    <row r="130" spans="1:16">
+    <row r="130" spans="1:16" hidden="true">
       <c r="A130" s="43"/>
       <c r="B130" s="46"/>
       <c r="C130" s="47"/>
@@ -3856,7 +3545,7 @@
       <c r="O130" s="47"/>
       <c r="P130" s="44"/>
     </row>
-    <row r="131" spans="1:16">
+    <row r="131" spans="1:16" hidden="true">
       <c r="A131" s="43"/>
       <c r="B131" s="46"/>
       <c r="C131" s="47"/>
@@ -3874,7 +3563,7 @@
       <c r="O131" s="47"/>
       <c r="P131" s="44"/>
     </row>
-    <row r="132" spans="1:16">
+    <row r="132" spans="1:16" hidden="true">
       <c r="A132" s="43"/>
       <c r="B132" s="46"/>
       <c r="C132" s="47"/>
@@ -3892,7 +3581,7 @@
       <c r="O132" s="47"/>
       <c r="P132" s="44"/>
     </row>
-    <row r="133" spans="1:16">
+    <row r="133" spans="1:16" hidden="true">
       <c r="A133" s="43"/>
       <c r="B133" s="46"/>
       <c r="C133" s="47"/>
@@ -3910,7 +3599,7 @@
       <c r="O133" s="47"/>
       <c r="P133" s="44"/>
     </row>
-    <row r="134" spans="1:16">
+    <row r="134" spans="1:16" hidden="true">
       <c r="A134" s="43"/>
       <c r="B134" s="46"/>
       <c r="C134" s="47"/>
@@ -3928,7 +3617,7 @@
       <c r="O134" s="47"/>
       <c r="P134" s="44"/>
     </row>
-    <row r="135" spans="1:16">
+    <row r="135" spans="1:16" hidden="true">
       <c r="A135" s="49"/>
       <c r="B135" s="49"/>
       <c r="C135" s="47"/>

</xml_diff>

<commit_message>
fix para anho en reporte
</commit_message>
<xml_diff>
--- a/public_html/admin/reportesgenerados/EnrollmentFees-87.xlsx
+++ b/public_html/admin/reportesgenerados/EnrollmentFees-87.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="115">
   <si>
     <r>
       <t xml:space="preserve">Renaissance</t>
@@ -55,7 +55,7 @@
     <t>Reflects "Received Revenues" thru:</t>
   </si>
   <si>
-    <t>06/16/2017</t>
+    <t>12/31/2017</t>
   </si>
   <si>
     <t>Enrollment Fees</t>
@@ -147,6 +147,117 @@
     <t>Amount</t>
   </si>
   <si>
+    <t>PE-01-02-53</t>
+  </si>
+  <si>
+    <t>01/27/2017</t>
+  </si>
+  <si>
+    <t>PE-01-04-29</t>
+  </si>
+  <si>
+    <t>02/22/2017</t>
+  </si>
+  <si>
+    <t>PE-01-05-27</t>
+  </si>
+  <si>
+    <t>03/24/2017</t>
+  </si>
+  <si>
+    <t>PE-01-02-54</t>
+  </si>
+  <si>
+    <t>04/19/2017</t>
+  </si>
+  <si>
+    <t>PE-01-06-22</t>
+  </si>
+  <si>
+    <t>02/01/2017</t>
+  </si>
+  <si>
+    <t>PE-01-06-23</t>
+  </si>
+  <si>
+    <t>PE-01-06-26</t>
+  </si>
+  <si>
+    <t>04/21/2017</t>
+  </si>
+  <si>
+    <t>PE-01-07-17</t>
+  </si>
+  <si>
+    <t>02/23/2017</t>
+  </si>
+  <si>
+    <t>PE-01-06-24</t>
+  </si>
+  <si>
+    <t>03/01/2017</t>
+  </si>
+  <si>
+    <t>PE-01-10-06</t>
+  </si>
+  <si>
+    <t>04/18/2017</t>
+  </si>
+  <si>
+    <t>PE-01-08-16</t>
+  </si>
+  <si>
+    <t>PE-01-07-22</t>
+  </si>
+  <si>
+    <t>03/16/2017</t>
+  </si>
+  <si>
+    <t>PE-01-08-17</t>
+  </si>
+  <si>
+    <t>02/24/2017</t>
+  </si>
+  <si>
+    <t>PE-01-07-26</t>
+  </si>
+  <si>
+    <t>03/23/2017</t>
+  </si>
+  <si>
+    <t>PE-01-09-12</t>
+  </si>
+  <si>
+    <t>02/20/2017</t>
+  </si>
+  <si>
+    <t>PE-01-10-08</t>
+  </si>
+  <si>
+    <t>03/02/2017</t>
+  </si>
+  <si>
+    <t>PE-01-10-01</t>
+  </si>
+  <si>
+    <t>02/17/2017</t>
+  </si>
+  <si>
+    <t>PE-01-10-02</t>
+  </si>
+  <si>
+    <t>02/13/2017</t>
+  </si>
+  <si>
+    <t>PE-01-10-04</t>
+  </si>
+  <si>
+    <t>02/14/2017</t>
+  </si>
+  <si>
+    <t>PE-01-10-05</t>
+  </si>
+  <si>
     <r>
       <t xml:space="preserve">TOTAL FOR </t>
     </r>
@@ -295,6 +406,87 @@
     </r>
   </si>
   <si>
+    <t>PE-01-01-42</t>
+  </si>
+  <si>
+    <t>05/18/2017</t>
+  </si>
+  <si>
+    <t>PE-01-08-18</t>
+  </si>
+  <si>
+    <t>06/23/2017</t>
+  </si>
+  <si>
+    <t>PE-01-01-43</t>
+  </si>
+  <si>
+    <t>07/15/2017</t>
+  </si>
+  <si>
+    <t>PE-01-01-44</t>
+  </si>
+  <si>
+    <t>08/18/2017</t>
+  </si>
+  <si>
+    <t>PE-01-04-30</t>
+  </si>
+  <si>
+    <t>05/24/2017</t>
+  </si>
+  <si>
+    <t>PE-01-09-13</t>
+  </si>
+  <si>
+    <t>06/13/2017</t>
+  </si>
+  <si>
+    <t>PE-01-07-27</t>
+  </si>
+  <si>
+    <t>07/11/2017</t>
+  </si>
+  <si>
+    <t>PE-01-04-31</t>
+  </si>
+  <si>
+    <t>08/04/2017</t>
+  </si>
+  <si>
+    <t>PE-01-07-29</t>
+  </si>
+  <si>
+    <t>05/23/2017</t>
+  </si>
+  <si>
+    <t>PE-01-09-05</t>
+  </si>
+  <si>
+    <t>07/07/2017</t>
+  </si>
+  <si>
+    <t>PE-01-10-09</t>
+  </si>
+  <si>
+    <t>05/05/2017</t>
+  </si>
+  <si>
+    <t>PE-01-10-14</t>
+  </si>
+  <si>
+    <t>07/24/2017</t>
+  </si>
+  <si>
+    <t>PE-01-10-10</t>
+  </si>
+  <si>
+    <t>05/04/2017</t>
+  </si>
+  <si>
+    <t>PE-01-10-11</t>
+  </si>
+  <si>
     <r>
       <t xml:space="preserve">TOTAL FOR </t>
     </r>
@@ -429,6 +621,51 @@
       </rPr>
       <t xml:space="preserve">DECEMBER</t>
     </r>
+  </si>
+  <si>
+    <t>PE-01-01-45</t>
+  </si>
+  <si>
+    <t>09/05/2017</t>
+  </si>
+  <si>
+    <t>PE-01-10-13</t>
+  </si>
+  <si>
+    <t>10/10/2017</t>
+  </si>
+  <si>
+    <t>PE-01-11-03</t>
+  </si>
+  <si>
+    <t>09/29/2017</t>
+  </si>
+  <si>
+    <t>PE-01-11-02</t>
+  </si>
+  <si>
+    <t>10/11/2017</t>
+  </si>
+  <si>
+    <t>PE-01-11-05</t>
+  </si>
+  <si>
+    <t>10/03/2017</t>
+  </si>
+  <si>
+    <t>PE-01-11-11</t>
+  </si>
+  <si>
+    <t>10/06/2017</t>
+  </si>
+  <si>
+    <t>PE-01-12-04</t>
+  </si>
+  <si>
+    <t>10/26/2017</t>
+  </si>
+  <si>
+    <t>PE-01-12-06</t>
   </si>
   <si>
     <r>
@@ -1548,57 +1785,129 @@
       </c>
     </row>
     <row r="10" spans="1:16">
-      <c r="A10" s="12"/>
-      <c r="B10" s="13"/>
-      <c r="C10" s="14"/>
-      <c r="E10" s="12"/>
-      <c r="F10" s="13"/>
-      <c r="G10" s="14"/>
-      <c r="I10" s="12"/>
-      <c r="J10" s="13"/>
-      <c r="K10" s="14"/>
-      <c r="M10" s="12"/>
-      <c r="N10" s="13"/>
-      <c r="O10" s="14"/>
+      <c r="A10" s="12" t="s">
+        <v>16</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>17</v>
+      </c>
+      <c r="C10" s="14">
+        <v>740</v>
+      </c>
+      <c r="E10" s="12" t="s">
+        <v>18</v>
+      </c>
+      <c r="F10" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="G10" s="14">
+        <v>780</v>
+      </c>
+      <c r="I10" s="12" t="s">
+        <v>20</v>
+      </c>
+      <c r="J10" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="K10" s="14">
+        <v>780</v>
+      </c>
+      <c r="M10" s="12" t="s">
+        <v>22</v>
+      </c>
+      <c r="N10" s="13" t="s">
+        <v>23</v>
+      </c>
+      <c r="O10" s="14">
+        <v>780</v>
+      </c>
     </row>
     <row r="11" spans="1:16">
       <c r="A11" s="15"/>
       <c r="B11" s="16"/>
       <c r="C11" s="14"/>
-      <c r="E11" s="12"/>
-      <c r="F11" s="13"/>
-      <c r="G11" s="14"/>
-      <c r="I11" s="12"/>
-      <c r="J11" s="13"/>
-      <c r="K11" s="14"/>
-      <c r="M11" s="12"/>
-      <c r="N11" s="13"/>
-      <c r="O11" s="14"/>
+      <c r="E11" s="12" t="s">
+        <v>24</v>
+      </c>
+      <c r="F11" s="13" t="s">
+        <v>25</v>
+      </c>
+      <c r="G11" s="14">
+        <v>740</v>
+      </c>
+      <c r="I11" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="J11" s="13" t="s">
+        <v>21</v>
+      </c>
+      <c r="K11" s="14">
+        <v>780</v>
+      </c>
+      <c r="M11" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="N11" s="13" t="s">
+        <v>28</v>
+      </c>
+      <c r="O11" s="14">
+        <v>780</v>
+      </c>
     </row>
     <row r="12" spans="1:16">
       <c r="A12" s="15"/>
       <c r="B12" s="16"/>
       <c r="C12" s="14"/>
-      <c r="E12" s="12"/>
-      <c r="F12" s="16"/>
-      <c r="G12" s="14"/>
-      <c r="I12" s="12"/>
-      <c r="J12" s="13"/>
-      <c r="K12" s="14"/>
-      <c r="M12" s="12"/>
-      <c r="N12" s="13"/>
-      <c r="O12" s="14"/>
+      <c r="E12" s="12" t="s">
+        <v>29</v>
+      </c>
+      <c r="F12" s="16" t="s">
+        <v>30</v>
+      </c>
+      <c r="G12" s="14">
+        <v>740</v>
+      </c>
+      <c r="I12" s="12" t="s">
+        <v>31</v>
+      </c>
+      <c r="J12" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="K12" s="14">
+        <v>780</v>
+      </c>
+      <c r="M12" s="12" t="s">
+        <v>33</v>
+      </c>
+      <c r="N12" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="O12" s="14">
+        <v>740</v>
+      </c>
     </row>
     <row r="13" spans="1:16">
       <c r="A13" s="15"/>
       <c r="B13" s="16"/>
       <c r="C13" s="17"/>
-      <c r="E13" s="12"/>
-      <c r="F13" s="16"/>
-      <c r="G13" s="17"/>
-      <c r="I13" s="12"/>
-      <c r="J13" s="13"/>
-      <c r="K13" s="17"/>
+      <c r="E13" s="12" t="s">
+        <v>35</v>
+      </c>
+      <c r="F13" s="16" t="s">
+        <v>25</v>
+      </c>
+      <c r="G13" s="17">
+        <v>740</v>
+      </c>
+      <c r="I13" s="12" t="s">
+        <v>36</v>
+      </c>
+      <c r="J13" s="13" t="s">
+        <v>37</v>
+      </c>
+      <c r="K13" s="17">
+        <v>740</v>
+      </c>
       <c r="M13" s="15"/>
       <c r="N13" s="16"/>
       <c r="O13" s="17"/>
@@ -1607,12 +1916,24 @@
       <c r="A14" s="15"/>
       <c r="B14" s="16"/>
       <c r="C14" s="14"/>
-      <c r="E14" s="15"/>
-      <c r="F14" s="16"/>
-      <c r="G14" s="14"/>
-      <c r="I14" s="15"/>
-      <c r="J14" s="18"/>
-      <c r="K14" s="14"/>
+      <c r="E14" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="F14" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="G14" s="14">
+        <v>780</v>
+      </c>
+      <c r="I14" s="15" t="s">
+        <v>40</v>
+      </c>
+      <c r="J14" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="K14" s="14">
+        <v>740</v>
+      </c>
       <c r="M14" s="15"/>
       <c r="N14" s="16"/>
       <c r="O14" s="14"/>
@@ -1621,12 +1942,24 @@
       <c r="A15" s="15"/>
       <c r="B15" s="16"/>
       <c r="C15" s="14"/>
-      <c r="E15" s="15"/>
-      <c r="F15" s="16"/>
-      <c r="G15" s="14"/>
-      <c r="I15" s="15"/>
-      <c r="J15" s="18"/>
-      <c r="K15" s="14"/>
+      <c r="E15" s="15" t="s">
+        <v>42</v>
+      </c>
+      <c r="F15" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="G15" s="14">
+        <v>740</v>
+      </c>
+      <c r="I15" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="J15" s="18" t="s">
+        <v>45</v>
+      </c>
+      <c r="K15" s="14">
+        <v>520</v>
+      </c>
       <c r="M15" s="15"/>
       <c r="N15" s="16"/>
       <c r="O15" s="14"/>
@@ -1635,9 +1968,15 @@
       <c r="A16" s="15"/>
       <c r="B16" s="16"/>
       <c r="C16" s="17"/>
-      <c r="E16" s="15"/>
-      <c r="F16" s="16"/>
-      <c r="G16" s="17"/>
+      <c r="E16" s="15" t="s">
+        <v>46</v>
+      </c>
+      <c r="F16" s="16" t="s">
+        <v>47</v>
+      </c>
+      <c r="G16" s="17">
+        <v>780</v>
+      </c>
       <c r="I16" s="15"/>
       <c r="J16" s="16"/>
       <c r="K16" s="17"/>
@@ -1649,9 +1988,15 @@
       <c r="A17" s="19"/>
       <c r="B17" s="20"/>
       <c r="C17" s="21"/>
-      <c r="E17" s="19"/>
-      <c r="F17" s="20"/>
-      <c r="G17" s="21"/>
+      <c r="E17" s="19" t="s">
+        <v>48</v>
+      </c>
+      <c r="F17" s="20" t="s">
+        <v>49</v>
+      </c>
+      <c r="G17" s="21">
+        <v>780</v>
+      </c>
       <c r="I17" s="19"/>
       <c r="J17" s="20"/>
       <c r="K17" s="21"/>
@@ -1663,9 +2008,15 @@
       <c r="A18" s="19"/>
       <c r="B18" s="20"/>
       <c r="C18" s="21"/>
-      <c r="E18" s="19"/>
-      <c r="F18" s="20"/>
-      <c r="G18" s="21"/>
+      <c r="E18" s="19" t="s">
+        <v>50</v>
+      </c>
+      <c r="F18" s="20" t="s">
+        <v>51</v>
+      </c>
+      <c r="G18" s="21">
+        <v>780</v>
+      </c>
       <c r="I18" s="19"/>
       <c r="J18" s="20"/>
       <c r="K18" s="21"/>
@@ -1677,9 +2028,15 @@
       <c r="A19" s="19"/>
       <c r="B19" s="20"/>
       <c r="C19" s="21"/>
-      <c r="E19" s="19"/>
-      <c r="F19" s="20"/>
-      <c r="G19" s="21"/>
+      <c r="E19" s="19" t="s">
+        <v>52</v>
+      </c>
+      <c r="F19" s="20" t="s">
+        <v>39</v>
+      </c>
+      <c r="G19" s="21">
+        <v>780</v>
+      </c>
       <c r="I19" s="19"/>
       <c r="J19" s="20"/>
       <c r="K19" s="21"/>
@@ -1773,7 +2130,7 @@
     </row>
     <row r="26" spans="1:16" customHeight="1" ht="17.25">
       <c r="A26" s="36" t="s">
-        <v>16</v>
+        <v>53</v>
       </c>
       <c r="B26" s="37"/>
       <c r="C26" s="25" t="str">
@@ -1781,7 +2138,7 @@
         <v>0</v>
       </c>
       <c r="E26" s="38" t="s">
-        <v>17</v>
+        <v>54</v>
       </c>
       <c r="F26" s="38"/>
       <c r="G26" s="25" t="str">
@@ -1789,7 +2146,7 @@
         <v>0</v>
       </c>
       <c r="I26" s="36" t="s">
-        <v>18</v>
+        <v>55</v>
       </c>
       <c r="J26" s="36"/>
       <c r="K26" s="25" t="str">
@@ -1797,7 +2154,7 @@
         <v>0</v>
       </c>
       <c r="M26" s="36" t="s">
-        <v>19</v>
+        <v>56</v>
       </c>
       <c r="N26" s="36"/>
       <c r="O26" s="25" t="str">
@@ -1808,22 +2165,22 @@
     <row r="27" spans="1:16" customHeight="1" ht="17.25"/>
     <row r="28" spans="1:16" customHeight="1" ht="17.25">
       <c r="A28" s="33" t="s">
-        <v>20</v>
+        <v>57</v>
       </c>
       <c r="B28" s="34"/>
       <c r="C28" s="35"/>
       <c r="E28" s="33" t="s">
-        <v>21</v>
+        <v>58</v>
       </c>
       <c r="F28" s="34"/>
       <c r="G28" s="35"/>
       <c r="I28" s="33" t="s">
-        <v>22</v>
+        <v>59</v>
       </c>
       <c r="J28" s="34"/>
       <c r="K28" s="35"/>
       <c r="M28" s="33" t="s">
-        <v>23</v>
+        <v>60</v>
       </c>
       <c r="N28" s="34"/>
       <c r="O28" s="35"/>
@@ -1905,65 +2262,143 @@
       </c>
     </row>
     <row r="31" spans="1:16">
-      <c r="A31" s="12"/>
-      <c r="B31" s="13"/>
-      <c r="C31" s="14"/>
-      <c r="E31" s="12"/>
-      <c r="F31" s="13"/>
-      <c r="G31" s="14"/>
-      <c r="I31" s="12"/>
-      <c r="J31" s="13"/>
-      <c r="K31" s="14"/>
-      <c r="M31" s="12"/>
-      <c r="N31" s="13"/>
-      <c r="O31" s="14"/>
+      <c r="A31" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="B31" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="C31" s="14">
+        <v>780</v>
+      </c>
+      <c r="E31" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="F31" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="G31" s="14">
+        <v>780</v>
+      </c>
+      <c r="I31" s="12" t="s">
+        <v>65</v>
+      </c>
+      <c r="J31" s="13" t="s">
+        <v>66</v>
+      </c>
+      <c r="K31" s="14">
+        <v>780</v>
+      </c>
+      <c r="M31" s="12" t="s">
+        <v>67</v>
+      </c>
+      <c r="N31" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="O31" s="14">
+        <v>780</v>
+      </c>
     </row>
     <row r="32" spans="1:16">
-      <c r="A32" s="12"/>
-      <c r="B32" s="13"/>
-      <c r="C32" s="14"/>
-      <c r="E32" s="12"/>
-      <c r="F32" s="13"/>
-      <c r="G32" s="14"/>
-      <c r="I32" s="12"/>
-      <c r="J32" s="13"/>
-      <c r="K32" s="14"/>
-      <c r="M32" s="26"/>
-      <c r="N32" s="13"/>
-      <c r="O32" s="14"/>
+      <c r="A32" s="12" t="s">
+        <v>69</v>
+      </c>
+      <c r="B32" s="13" t="s">
+        <v>70</v>
+      </c>
+      <c r="C32" s="14">
+        <v>780</v>
+      </c>
+      <c r="E32" s="12" t="s">
+        <v>71</v>
+      </c>
+      <c r="F32" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="G32" s="14">
+        <v>780</v>
+      </c>
+      <c r="I32" s="12" t="s">
+        <v>73</v>
+      </c>
+      <c r="J32" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="K32" s="14">
+        <v>780</v>
+      </c>
+      <c r="M32" s="26" t="s">
+        <v>75</v>
+      </c>
+      <c r="N32" s="13" t="s">
+        <v>76</v>
+      </c>
+      <c r="O32" s="14">
+        <v>780</v>
+      </c>
     </row>
     <row r="33" spans="1:16">
-      <c r="A33" s="12"/>
-      <c r="B33" s="13"/>
-      <c r="C33" s="14"/>
+      <c r="A33" s="12" t="s">
+        <v>77</v>
+      </c>
+      <c r="B33" s="13" t="s">
+        <v>78</v>
+      </c>
+      <c r="C33" s="14">
+        <v>780</v>
+      </c>
       <c r="E33" s="26"/>
       <c r="F33" s="13"/>
       <c r="G33" s="14"/>
-      <c r="I33" s="12"/>
-      <c r="J33" s="13"/>
-      <c r="K33" s="14"/>
+      <c r="I33" s="12" t="s">
+        <v>79</v>
+      </c>
+      <c r="J33" s="13" t="s">
+        <v>80</v>
+      </c>
+      <c r="K33" s="14">
+        <v>740</v>
+      </c>
       <c r="M33" s="26"/>
       <c r="N33" s="13"/>
       <c r="O33" s="14"/>
     </row>
     <row r="34" spans="1:16">
-      <c r="A34" s="15"/>
-      <c r="B34" s="16"/>
-      <c r="C34" s="17"/>
+      <c r="A34" s="15" t="s">
+        <v>81</v>
+      </c>
+      <c r="B34" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="C34" s="17">
+        <v>780</v>
+      </c>
       <c r="E34" s="15"/>
       <c r="F34" s="16"/>
       <c r="G34" s="17"/>
-      <c r="I34" s="12"/>
-      <c r="J34" s="13"/>
-      <c r="K34" s="14"/>
+      <c r="I34" s="12" t="s">
+        <v>83</v>
+      </c>
+      <c r="J34" s="13" t="s">
+        <v>84</v>
+      </c>
+      <c r="K34" s="14">
+        <v>780</v>
+      </c>
       <c r="M34" s="15"/>
       <c r="N34" s="13"/>
       <c r="O34" s="17"/>
     </row>
     <row r="35" spans="1:16">
-      <c r="A35" s="15"/>
-      <c r="B35" s="16"/>
-      <c r="C35" s="14"/>
+      <c r="A35" s="15" t="s">
+        <v>85</v>
+      </c>
+      <c r="B35" s="16" t="s">
+        <v>86</v>
+      </c>
+      <c r="C35" s="14">
+        <v>780</v>
+      </c>
       <c r="E35" s="26"/>
       <c r="F35" s="13"/>
       <c r="G35" s="14"/>
@@ -1975,9 +2410,15 @@
       <c r="O35" s="14"/>
     </row>
     <row r="36" spans="1:16">
-      <c r="A36" s="15"/>
-      <c r="B36" s="16"/>
-      <c r="C36" s="14"/>
+      <c r="A36" s="15" t="s">
+        <v>87</v>
+      </c>
+      <c r="B36" s="16" t="s">
+        <v>82</v>
+      </c>
+      <c r="C36" s="14">
+        <v>780</v>
+      </c>
       <c r="E36" s="26"/>
       <c r="F36" s="13"/>
       <c r="G36" s="14"/>
@@ -2130,7 +2571,7 @@
     </row>
     <row r="47" spans="1:16" customHeight="1" ht="17.25">
       <c r="A47" s="36" t="s">
-        <v>24</v>
+        <v>88</v>
       </c>
       <c r="B47" s="36"/>
       <c r="C47" s="25" t="str">
@@ -2138,7 +2579,7 @@
         <v>0</v>
       </c>
       <c r="E47" s="36" t="s">
-        <v>25</v>
+        <v>89</v>
       </c>
       <c r="F47" s="36"/>
       <c r="G47" s="25" t="str">
@@ -2146,7 +2587,7 @@
         <v>0</v>
       </c>
       <c r="I47" s="36" t="s">
-        <v>26</v>
+        <v>90</v>
       </c>
       <c r="J47" s="36"/>
       <c r="K47" s="25" t="str">
@@ -2154,7 +2595,7 @@
         <v>0</v>
       </c>
       <c r="M47" s="36" t="s">
-        <v>27</v>
+        <v>91</v>
       </c>
       <c r="N47" s="36"/>
       <c r="O47" s="25" t="str">
@@ -2165,22 +2606,22 @@
     <row r="48" spans="1:16" customHeight="1" ht="17.25"/>
     <row r="49" spans="1:16" customHeight="1" ht="17.25">
       <c r="A49" s="33" t="s">
-        <v>28</v>
+        <v>92</v>
       </c>
       <c r="B49" s="34"/>
       <c r="C49" s="35"/>
       <c r="E49" s="33" t="s">
-        <v>29</v>
+        <v>93</v>
       </c>
       <c r="F49" s="34"/>
       <c r="G49" s="35"/>
       <c r="I49" s="33" t="s">
-        <v>30</v>
+        <v>94</v>
       </c>
       <c r="J49" s="34"/>
       <c r="K49" s="35"/>
       <c r="M49" s="33" t="s">
-        <v>31</v>
+        <v>95</v>
       </c>
       <c r="N49" s="34"/>
       <c r="O49" s="35"/>
@@ -2262,12 +2703,24 @@
       </c>
     </row>
     <row r="52" spans="1:16">
-      <c r="A52" s="12"/>
-      <c r="B52" s="13"/>
-      <c r="C52" s="14"/>
-      <c r="E52" s="12"/>
-      <c r="F52" s="13"/>
-      <c r="G52" s="14"/>
+      <c r="A52" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="B52" s="13" t="s">
+        <v>97</v>
+      </c>
+      <c r="C52" s="14">
+        <v>780</v>
+      </c>
+      <c r="E52" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="F52" s="13" t="s">
+        <v>99</v>
+      </c>
+      <c r="G52" s="14">
+        <v>780</v>
+      </c>
       <c r="I52" s="12"/>
       <c r="J52" s="13"/>
       <c r="K52" s="14"/>
@@ -2276,12 +2729,24 @@
       <c r="O52" s="14"/>
     </row>
     <row r="53" spans="1:16">
-      <c r="A53" s="12"/>
-      <c r="B53" s="13"/>
-      <c r="C53" s="14"/>
-      <c r="E53" s="12"/>
-      <c r="F53" s="13"/>
-      <c r="G53" s="14"/>
+      <c r="A53" s="12" t="s">
+        <v>100</v>
+      </c>
+      <c r="B53" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="C53" s="14">
+        <v>780</v>
+      </c>
+      <c r="E53" s="12" t="s">
+        <v>102</v>
+      </c>
+      <c r="F53" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="G53" s="14">
+        <v>390</v>
+      </c>
       <c r="I53" s="12"/>
       <c r="J53" s="18"/>
       <c r="K53" s="14"/>
@@ -2293,9 +2758,15 @@
       <c r="A54" s="15"/>
       <c r="B54" s="13"/>
       <c r="C54" s="14"/>
-      <c r="E54" s="12"/>
-      <c r="F54" s="13"/>
-      <c r="G54" s="14"/>
+      <c r="E54" s="12" t="s">
+        <v>104</v>
+      </c>
+      <c r="F54" s="13" t="s">
+        <v>105</v>
+      </c>
+      <c r="G54" s="14">
+        <v>780</v>
+      </c>
       <c r="I54" s="12"/>
       <c r="J54" s="18"/>
       <c r="K54" s="14"/>
@@ -2307,9 +2778,15 @@
       <c r="A55" s="15"/>
       <c r="B55" s="13"/>
       <c r="C55" s="17"/>
-      <c r="E55" s="12"/>
-      <c r="F55" s="13"/>
-      <c r="G55" s="17"/>
+      <c r="E55" s="12" t="s">
+        <v>106</v>
+      </c>
+      <c r="F55" s="13" t="s">
+        <v>107</v>
+      </c>
+      <c r="G55" s="17">
+        <v>390</v>
+      </c>
       <c r="I55" s="12"/>
       <c r="J55" s="18"/>
       <c r="K55" s="17"/>
@@ -2321,9 +2798,15 @@
       <c r="A56" s="15"/>
       <c r="B56" s="13"/>
       <c r="C56" s="14"/>
-      <c r="E56" s="15"/>
-      <c r="F56" s="13"/>
-      <c r="G56" s="14"/>
+      <c r="E56" s="15" t="s">
+        <v>108</v>
+      </c>
+      <c r="F56" s="13" t="s">
+        <v>109</v>
+      </c>
+      <c r="G56" s="14">
+        <v>780</v>
+      </c>
       <c r="I56" s="15"/>
       <c r="J56" s="18"/>
       <c r="K56" s="14"/>
@@ -2335,9 +2818,15 @@
       <c r="A57" s="15"/>
       <c r="B57" s="13"/>
       <c r="C57" s="14"/>
-      <c r="E57" s="15"/>
-      <c r="F57" s="16"/>
-      <c r="G57" s="14"/>
+      <c r="E57" s="15" t="s">
+        <v>110</v>
+      </c>
+      <c r="F57" s="16" t="s">
+        <v>109</v>
+      </c>
+      <c r="G57" s="14">
+        <v>780</v>
+      </c>
       <c r="I57" s="15"/>
       <c r="J57" s="18"/>
       <c r="K57" s="14"/>
@@ -2487,7 +2976,7 @@
     </row>
     <row r="68" spans="1:16" customHeight="1" ht="17.25">
       <c r="A68" s="36" t="s">
-        <v>32</v>
+        <v>111</v>
       </c>
       <c r="B68" s="36"/>
       <c r="C68" s="25" t="str">
@@ -2495,7 +2984,7 @@
         <v>0</v>
       </c>
       <c r="E68" s="36" t="s">
-        <v>33</v>
+        <v>112</v>
       </c>
       <c r="F68" s="36"/>
       <c r="G68" s="25" t="str">
@@ -2503,7 +2992,7 @@
         <v>0</v>
       </c>
       <c r="I68" s="36" t="s">
-        <v>34</v>
+        <v>113</v>
       </c>
       <c r="J68" s="36"/>
       <c r="K68" s="25" t="str">
@@ -2511,7 +3000,7 @@
         <v>0</v>
       </c>
       <c r="M68" s="36" t="s">
-        <v>35</v>
+        <v>114</v>
       </c>
       <c r="N68" s="36"/>
       <c r="O68" s="25" t="str">
@@ -2522,7 +3011,7 @@
     <row r="71" spans="1:16" customHeight="1" ht="17.25"/>
     <row r="72" spans="1:16" customHeight="1" ht="27.75">
       <c r="A72" s="39">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="B72" s="40"/>
       <c r="C72" s="40"/>
@@ -2864,7 +3353,7 @@
     </row>
     <row r="93" spans="1:16" customHeight="1" ht="17.25">
       <c r="A93" s="36" t="s">
-        <v>16</v>
+        <v>53</v>
       </c>
       <c r="B93" s="36"/>
       <c r="C93" s="25" t="str">
@@ -2872,7 +3361,7 @@
         <v>0</v>
       </c>
       <c r="E93" s="38" t="s">
-        <v>17</v>
+        <v>54</v>
       </c>
       <c r="F93" s="38"/>
       <c r="G93" s="25" t="str">
@@ -2880,7 +3369,7 @@
         <v>0</v>
       </c>
       <c r="I93" s="36" t="s">
-        <v>18</v>
+        <v>55</v>
       </c>
       <c r="J93" s="36"/>
       <c r="K93" s="25" t="str">
@@ -2888,7 +3377,7 @@
         <v>0</v>
       </c>
       <c r="M93" s="36" t="s">
-        <v>19</v>
+        <v>56</v>
       </c>
       <c r="N93" s="36"/>
       <c r="O93" s="25" t="str">

</xml_diff>